<commit_message>
Update homeless population by categories.xlsx
</commit_message>
<xml_diff>
--- a/Data/homeless population by categories.xlsx
+++ b/Data/homeless population by categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/GitHub/Homelessness-Final-Group-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{D3BC0822-C516-4101-81AF-F58D69EE6760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E5827F9-BEFD-4791-ABE2-86CE254A33A5}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{D3BC0822-C516-4101-81AF-F58D69EE6760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50DBCC7D-6948-4F81-82CF-C34E743F6E47}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">    By age</t>
   </si>
@@ -91,10 +91,16 @@
     <t>Unsheltered total</t>
   </si>
   <si>
-    <t xml:space="preserve">Individuals  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">People in families with children </t>
+    <t xml:space="preserve">unshelter Individuals  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unshelter People in families with children </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelter Individuals  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelter People in families with children </t>
   </si>
 </sst>
 </file>
@@ -938,7 +944,7 @@
   <dimension ref="A1:AW8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1365,7 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1475,7 +1481,7 @@
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>